<commit_message>
Fixes made to: hydro with dam, fuel links,
</commit_message>
<xml_diff>
--- a/KENTIM/DataSpreadsheets/Demand_LossesCalibration.xlsx
+++ b/KENTIM/DataSpreadsheets/Demand_LossesCalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\KENTIMGE\KENTIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19903BBC-642F-4000-8408-3DC14EE870D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162307BF-8D59-4813-BC38-4192E2238362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{D3248BDD-D506-434D-BF3B-2641FA8A22D5}"/>
+    <workbookView xWindow="2565" yWindow="150" windowWidth="26235" windowHeight="15450" xr2:uid="{D3248BDD-D506-434D-BF3B-2641FA8A22D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,10 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5D5AA5-2C01-4EFF-BE18-53D73F0EEC23}">
-  <dimension ref="A1:AM23"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AM27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A11:A13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +534,12 @@
         <v>7.5232999999999999</v>
       </c>
     </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>SUM(D2:D4)/3.6</f>
+        <v>10.781111111111111</v>
+      </c>
+    </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
@@ -609,6 +616,10 @@
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>D5/D8</f>
+        <v>0.9</v>
+      </c>
       <c r="I9">
         <v>12.07</v>
       </c>
@@ -1067,8 +1078,20 @@
         <v>10.432098765432096</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" ref="I16" si="8">SUM(I10:I12)/I14/I15/3.6</f>
-        <v>12.016830694622737</v>
+        <f>SUM(I11:I13)/I14/I15/3.6</f>
+        <v>14.940807302809873</v>
+      </c>
+    </row>
+    <row r="17" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>I14*I15</f>
+        <v>0.77899999999999991</v>
+      </c>
+    </row>
+    <row r="18" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f>1-I17</f>
+        <v>0.22100000000000009</v>
       </c>
     </row>
     <row r="20" spans="3:39" x14ac:dyDescent="0.25">
@@ -1506,6 +1529,28 @@
       </c>
       <c r="AM23">
         <v>109.3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f>SUM(I21:I23)</f>
+        <v>41.9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f>H16*(1-0.23)</f>
+        <v>8.0327160493827137</v>
+      </c>
+      <c r="I26">
+        <f>H26*3.6</f>
+        <v>28.917777777777768</v>
+      </c>
+    </row>
+    <row r="27" spans="3:39" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f>I26/I25</f>
+        <v>0.69016176080615199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>